<commit_message>
fixed typo in test spreadsheet
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Fall2023/testfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Spring2024/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20FC16AB-1682-4235-BE05-82D5CA2CFDEB}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA45819-3BB0-47B9-BC1E-E197CD5BD143}"/>
   <bookViews>
-    <workbookView xWindow="-22860" yWindow="885" windowWidth="21735" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>test2.csv</t>
   </si>
   <si>
-    <t>Covariance with EW Variance (l=0.94), EW Correlation (l=0.97)</t>
-  </si>
-  <si>
     <t>near_psd covariance</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>VaR/ES on 2 levels from simulated values - Copula</t>
+  </si>
+  <si>
+    <t>Covariance with EW Variance (l=0.97), EW Correlation (l=0.94)</t>
   </si>
 </sst>
 </file>
@@ -496,18 +496,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -536,7 +536,7 @@
         <v>testout_1.1.csv</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -547,11 +547,11 @@
         <v>5</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D32" si="0">"testout_"&amp;A3&amp;".csv"</f>
+        <f t="shared" ref="D3:D30" si="0">"testout_"&amp;A3&amp;".csv"</f>
         <v>testout_1.2.csv</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -566,7 +566,7 @@
         <v>testout_1.3.csv</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -581,7 +581,7 @@
         <v>testout_1.4.csv</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.1</v>
       </c>
@@ -596,7 +596,7 @@
         <v>testout_2.1.csv</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -611,12 +611,12 @@
         <v>testout_2.2.csv</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.2999999999999998</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -626,330 +626,330 @@
         <v>testout_2.3.csv</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3.1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>testout_3.1.csv</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3.2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>testout_3.2.csv</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3.3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>testout_3.3.csv</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>testout_3.4.csv</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4.0999999999999996</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>testout_4.1.csv</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5.0999999999999996</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>testout_5.1.csv</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5.2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>testout_5.2.csv</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5.3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>testout_5.3.csv</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5.4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>testout_5.4.csv</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5.5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>testout_5.5.csv</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6.1</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>testout_6.1.csv</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>6.2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>testout_6.2.csv</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>7.1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>testout_7.1.csv</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>7.2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>testout_7.2.csv</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>7.3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>testout_7.3.csv</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>8.1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.1.csv</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8.1999999999999993</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.2.csv</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>8.3000000000000007</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.3.csv</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>8.4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.4.csv</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>8.5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.5.csv</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>8.6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.6.csv</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>9.1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>

</xml_diff>